<commit_message>
Updated Data with Alg Layer
</commit_message>
<xml_diff>
--- a/Data/Adjacency_Lists/All.xlsx
+++ b/Data/Adjacency_Lists/All.xlsx
@@ -8,33 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcoller/Box/ANCR/WAMV-Networks/multilayer_design_network_tool/Data/Adjacency_Lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C6CDDE-3E08-6C43-8332-37E84FBE3C53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCD6C60-1F27-4840-996F-A1D18ADB7D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29480" yWindow="1720" windowWidth="29180" windowHeight="19400" xr2:uid="{B91DE26E-70FB-D644-BC66-8F560A513936}"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -42,16 +29,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -59,15 +346,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -378,18 +854,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98BB2399-60BE-7242-BD6F-885036148CDE}">
-  <dimension ref="A1:Q212"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:EQ284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="A176" sqref="A176:J212"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="N278" sqref="N278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="17" width="5" customWidth="1"/>
-    <col min="18" max="31" width="4.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1">
@@ -2985,7 +3457,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>40</v>
       </c>
@@ -2993,17 +3465,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>41</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>43</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>44</v>
       </c>
@@ -3011,7 +3483,1996 @@
         <v>40</v>
       </c>
     </row>
+    <row r="213" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>111</v>
+      </c>
+      <c r="B213">
+        <v>55</v>
+      </c>
+      <c r="C213">
+        <v>56</v>
+      </c>
+      <c r="D213">
+        <v>53</v>
+      </c>
+      <c r="E213">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="214" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>57</v>
+      </c>
+      <c r="B214">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="215" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>58</v>
+      </c>
+      <c r="B215">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="216" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>126</v>
+      </c>
+      <c r="B216">
+        <v>57</v>
+      </c>
+      <c r="C216">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="217" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>59</v>
+      </c>
+      <c r="B217">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="218" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>60</v>
+      </c>
+      <c r="B218">
+        <v>124</v>
+      </c>
+      <c r="C218">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="219" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>61</v>
+      </c>
+      <c r="B219">
+        <v>124</v>
+      </c>
+      <c r="C219">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="220" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>62</v>
+      </c>
+      <c r="B220">
+        <v>124</v>
+      </c>
+      <c r="C220">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="221" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>64</v>
+      </c>
+      <c r="B221">
+        <v>103</v>
+      </c>
+      <c r="C221">
+        <v>104</v>
+      </c>
+      <c r="D221">
+        <v>105</v>
+      </c>
+      <c r="E221">
+        <v>106</v>
+      </c>
+      <c r="F221">
+        <v>107</v>
+      </c>
+      <c r="G221">
+        <v>108</v>
+      </c>
+      <c r="H221">
+        <v>109</v>
+      </c>
+      <c r="I221">
+        <v>110</v>
+      </c>
+      <c r="J221">
+        <v>111</v>
+      </c>
+      <c r="K221">
+        <v>112</v>
+      </c>
+      <c r="L221">
+        <v>113</v>
+      </c>
+      <c r="M221">
+        <v>114</v>
+      </c>
+      <c r="N221">
+        <v>115</v>
+      </c>
+      <c r="O221">
+        <v>116</v>
+      </c>
+      <c r="P221">
+        <v>117</v>
+      </c>
+      <c r="Q221">
+        <v>118</v>
+      </c>
+      <c r="R221">
+        <v>119</v>
+      </c>
+      <c r="S221">
+        <v>120</v>
+      </c>
+      <c r="T221">
+        <v>121</v>
+      </c>
+      <c r="U221">
+        <v>122</v>
+      </c>
+      <c r="V221">
+        <v>123</v>
+      </c>
+      <c r="W221">
+        <v>124</v>
+      </c>
+      <c r="X221">
+        <v>125</v>
+      </c>
+      <c r="Y221">
+        <v>126</v>
+      </c>
+      <c r="Z221">
+        <v>127</v>
+      </c>
+      <c r="AA221">
+        <v>128</v>
+      </c>
+      <c r="AB221">
+        <v>129</v>
+      </c>
+      <c r="AC221">
+        <v>130</v>
+      </c>
+      <c r="AD221">
+        <v>131</v>
+      </c>
+      <c r="AE221">
+        <v>132</v>
+      </c>
+      <c r="AF221">
+        <v>133</v>
+      </c>
+      <c r="AG221">
+        <v>134</v>
+      </c>
+      <c r="AH221">
+        <v>135</v>
+      </c>
+      <c r="AI221">
+        <v>136</v>
+      </c>
+      <c r="AJ221">
+        <v>137</v>
+      </c>
+      <c r="AK221">
+        <v>138</v>
+      </c>
+      <c r="AL221">
+        <v>139</v>
+      </c>
+      <c r="AM221">
+        <v>140</v>
+      </c>
+      <c r="AN221">
+        <v>141</v>
+      </c>
+      <c r="AO221">
+        <v>142</v>
+      </c>
+      <c r="AP221">
+        <v>143</v>
+      </c>
+      <c r="AQ221">
+        <v>144</v>
+      </c>
+      <c r="AR221">
+        <v>145</v>
+      </c>
+      <c r="AS221">
+        <v>146</v>
+      </c>
+      <c r="AT221">
+        <v>147</v>
+      </c>
+      <c r="AU221">
+        <v>148</v>
+      </c>
+      <c r="AV221">
+        <v>149</v>
+      </c>
+      <c r="AW221">
+        <v>150</v>
+      </c>
+      <c r="AX221">
+        <v>151</v>
+      </c>
+      <c r="AY221">
+        <v>152</v>
+      </c>
+      <c r="AZ221">
+        <v>153</v>
+      </c>
+      <c r="BA221">
+        <v>154</v>
+      </c>
+      <c r="BB221">
+        <v>155</v>
+      </c>
+      <c r="BC221">
+        <v>156</v>
+      </c>
+      <c r="BD221">
+        <v>157</v>
+      </c>
+      <c r="BE221">
+        <v>158</v>
+      </c>
+      <c r="BF221">
+        <v>159</v>
+      </c>
+      <c r="BG221">
+        <v>160</v>
+      </c>
+      <c r="BH221">
+        <v>161</v>
+      </c>
+      <c r="BI221">
+        <v>162</v>
+      </c>
+      <c r="BJ221">
+        <v>163</v>
+      </c>
+      <c r="BK221">
+        <v>164</v>
+      </c>
+      <c r="BL221">
+        <v>165</v>
+      </c>
+      <c r="BM221">
+        <v>166</v>
+      </c>
+      <c r="BN221">
+        <v>167</v>
+      </c>
+      <c r="BO221">
+        <v>168</v>
+      </c>
+      <c r="BP221">
+        <v>169</v>
+      </c>
+      <c r="BQ221">
+        <v>170</v>
+      </c>
+      <c r="BR221">
+        <v>171</v>
+      </c>
+      <c r="BS221">
+        <v>172</v>
+      </c>
+      <c r="BT221">
+        <v>173</v>
+      </c>
+      <c r="BU221">
+        <v>174</v>
+      </c>
+      <c r="BV221">
+        <v>175</v>
+      </c>
+      <c r="BW221">
+        <v>176</v>
+      </c>
+      <c r="BX221">
+        <v>177</v>
+      </c>
+      <c r="BY221">
+        <v>178</v>
+      </c>
+      <c r="BZ221">
+        <v>179</v>
+      </c>
+      <c r="CA221">
+        <v>180</v>
+      </c>
+      <c r="CB221">
+        <v>181</v>
+      </c>
+      <c r="CC221">
+        <v>182</v>
+      </c>
+      <c r="CD221">
+        <v>183</v>
+      </c>
+      <c r="CE221">
+        <v>184</v>
+      </c>
+      <c r="CF221">
+        <v>185</v>
+      </c>
+      <c r="CG221">
+        <v>186</v>
+      </c>
+      <c r="CH221">
+        <v>187</v>
+      </c>
+      <c r="CI221">
+        <v>188</v>
+      </c>
+      <c r="CJ221">
+        <v>189</v>
+      </c>
+      <c r="CK221">
+        <v>190</v>
+      </c>
+      <c r="CL221">
+        <v>191</v>
+      </c>
+      <c r="CM221">
+        <v>192</v>
+      </c>
+      <c r="CN221">
+        <v>193</v>
+      </c>
+      <c r="CO221">
+        <v>194</v>
+      </c>
+      <c r="CP221">
+        <v>195</v>
+      </c>
+      <c r="CQ221">
+        <v>196</v>
+      </c>
+      <c r="CR221">
+        <v>197</v>
+      </c>
+      <c r="CS221">
+        <v>198</v>
+      </c>
+      <c r="CT221">
+        <v>199</v>
+      </c>
+      <c r="CU221">
+        <v>200</v>
+      </c>
+      <c r="CV221">
+        <v>201</v>
+      </c>
+      <c r="CW221">
+        <v>202</v>
+      </c>
+      <c r="CX221">
+        <v>203</v>
+      </c>
+      <c r="CY221">
+        <v>204</v>
+      </c>
+      <c r="CZ221">
+        <v>205</v>
+      </c>
+      <c r="DA221">
+        <v>206</v>
+      </c>
+      <c r="DB221">
+        <v>207</v>
+      </c>
+      <c r="DC221">
+        <v>208</v>
+      </c>
+      <c r="DD221">
+        <v>209</v>
+      </c>
+      <c r="DE221">
+        <v>210</v>
+      </c>
+      <c r="DF221">
+        <v>211</v>
+      </c>
+      <c r="DG221">
+        <v>212</v>
+      </c>
+      <c r="DH221">
+        <v>213</v>
+      </c>
+      <c r="DI221">
+        <v>214</v>
+      </c>
+      <c r="DJ221">
+        <v>215</v>
+      </c>
+      <c r="DK221">
+        <v>216</v>
+      </c>
+      <c r="DL221">
+        <v>217</v>
+      </c>
+      <c r="DM221">
+        <v>218</v>
+      </c>
+      <c r="DN221">
+        <v>219</v>
+      </c>
+      <c r="DO221">
+        <v>220</v>
+      </c>
+      <c r="DP221">
+        <v>221</v>
+      </c>
+      <c r="DQ221">
+        <v>222</v>
+      </c>
+      <c r="DR221">
+        <v>223</v>
+      </c>
+      <c r="DS221">
+        <v>224</v>
+      </c>
+      <c r="DT221">
+        <v>225</v>
+      </c>
+      <c r="DU221">
+        <v>226</v>
+      </c>
+      <c r="DV221">
+        <v>227</v>
+      </c>
+      <c r="DW221">
+        <v>228</v>
+      </c>
+      <c r="DX221">
+        <v>229</v>
+      </c>
+      <c r="DY221">
+        <v>230</v>
+      </c>
+      <c r="DZ221">
+        <v>231</v>
+      </c>
+      <c r="EA221">
+        <v>232</v>
+      </c>
+      <c r="EB221">
+        <v>233</v>
+      </c>
+      <c r="EC221">
+        <v>234</v>
+      </c>
+      <c r="ED221">
+        <v>235</v>
+      </c>
+      <c r="EE221">
+        <v>236</v>
+      </c>
+      <c r="EF221">
+        <v>237</v>
+      </c>
+      <c r="EG221">
+        <v>238</v>
+      </c>
+      <c r="EH221">
+        <v>239</v>
+      </c>
+      <c r="EI221">
+        <v>240</v>
+      </c>
+      <c r="EJ221">
+        <v>241</v>
+      </c>
+      <c r="EK221">
+        <v>242</v>
+      </c>
+      <c r="EL221">
+        <v>243</v>
+      </c>
+      <c r="EM221">
+        <v>244</v>
+      </c>
+      <c r="EN221">
+        <v>245</v>
+      </c>
+      <c r="EO221">
+        <v>246</v>
+      </c>
+      <c r="EP221">
+        <v>247</v>
+      </c>
+      <c r="EQ221">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="222" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="223" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>122</v>
+      </c>
+      <c r="B223">
+        <v>141</v>
+      </c>
+      <c r="C223">
+        <v>123</v>
+      </c>
+      <c r="D223">
+        <v>170</v>
+      </c>
+      <c r="E223">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="224" spans="1:147" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>124</v>
+      </c>
+      <c r="B225">
+        <v>123</v>
+      </c>
+      <c r="C225">
+        <v>158</v>
+      </c>
+      <c r="D225">
+        <v>172</v>
+      </c>
+      <c r="E225">
+        <v>173</v>
+      </c>
+      <c r="F225">
+        <v>174</v>
+      </c>
+      <c r="G225">
+        <v>170</v>
+      </c>
+      <c r="H225">
+        <v>175</v>
+      </c>
+      <c r="I225">
+        <v>176</v>
+      </c>
+      <c r="J225">
+        <v>121</v>
+      </c>
+      <c r="K225">
+        <v>145</v>
+      </c>
+      <c r="L225">
+        <v>141</v>
+      </c>
+      <c r="M225">
+        <v>177</v>
+      </c>
+      <c r="N225">
+        <v>178</v>
+      </c>
+      <c r="O225">
+        <v>179</v>
+      </c>
+      <c r="P225">
+        <v>180</v>
+      </c>
+      <c r="Q225">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="226" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>125</v>
+      </c>
+      <c r="B226">
+        <v>178</v>
+      </c>
+      <c r="C226">
+        <v>182</v>
+      </c>
+      <c r="D226">
+        <v>158</v>
+      </c>
+      <c r="E226">
+        <v>141</v>
+      </c>
+      <c r="F226">
+        <v>183</v>
+      </c>
+      <c r="G226">
+        <v>179</v>
+      </c>
+      <c r="H226">
+        <v>184</v>
+      </c>
+      <c r="I226">
+        <v>168</v>
+      </c>
+      <c r="J226">
+        <v>185</v>
+      </c>
+      <c r="K226">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="227" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>126</v>
+      </c>
+      <c r="B227">
+        <v>179</v>
+      </c>
+      <c r="C227">
+        <v>186</v>
+      </c>
+      <c r="D227">
+        <v>166</v>
+      </c>
+      <c r="E227">
+        <v>187</v>
+      </c>
+      <c r="F227">
+        <v>171</v>
+      </c>
+      <c r="G227">
+        <v>181</v>
+      </c>
+      <c r="H227">
+        <v>188</v>
+      </c>
+      <c r="I227">
+        <v>178</v>
+      </c>
+      <c r="J227">
+        <v>189</v>
+      </c>
+      <c r="K227">
+        <v>190</v>
+      </c>
+      <c r="L227">
+        <v>141</v>
+      </c>
+      <c r="M227">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="228" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>159</v>
+      </c>
+      <c r="B228">
+        <v>178</v>
+      </c>
+      <c r="C228">
+        <v>175</v>
+      </c>
+      <c r="D228">
+        <v>141</v>
+      </c>
+      <c r="E228">
+        <v>155</v>
+      </c>
+      <c r="F228">
+        <v>123</v>
+      </c>
+      <c r="G228">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>127</v>
+      </c>
+      <c r="B229">
+        <v>166</v>
+      </c>
+      <c r="C229">
+        <v>187</v>
+      </c>
+      <c r="D229">
+        <v>171</v>
+      </c>
+      <c r="E229">
+        <v>188</v>
+      </c>
+      <c r="F229">
+        <v>191</v>
+      </c>
+      <c r="G229">
+        <v>192</v>
+      </c>
+      <c r="H229">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="230" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>128</v>
+      </c>
+      <c r="B230">
+        <v>137</v>
+      </c>
+      <c r="C230">
+        <v>158</v>
+      </c>
+      <c r="D230">
+        <v>119</v>
+      </c>
+      <c r="E230">
+        <v>106</v>
+      </c>
+      <c r="F230">
+        <v>193</v>
+      </c>
+      <c r="G230">
+        <v>194</v>
+      </c>
+      <c r="H230">
+        <v>195</v>
+      </c>
+      <c r="I230">
+        <v>196</v>
+      </c>
+      <c r="J230">
+        <v>197</v>
+      </c>
+      <c r="K230">
+        <v>198</v>
+      </c>
+      <c r="L230">
+        <v>199</v>
+      </c>
+      <c r="M230">
+        <v>180</v>
+      </c>
+      <c r="N230">
+        <v>200</v>
+      </c>
+      <c r="O230">
+        <v>201</v>
+      </c>
+      <c r="P230">
+        <v>179</v>
+      </c>
+      <c r="Q230">
+        <v>202</v>
+      </c>
+      <c r="R230">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="231" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>129</v>
+      </c>
+      <c r="B231">
+        <v>120</v>
+      </c>
+      <c r="C231">
+        <v>170</v>
+      </c>
+      <c r="D231">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="232" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>130</v>
+      </c>
+      <c r="B232">
+        <v>204</v>
+      </c>
+      <c r="C232">
+        <v>136</v>
+      </c>
+      <c r="D232">
+        <v>205</v>
+      </c>
+      <c r="E232">
+        <v>179</v>
+      </c>
+      <c r="F232">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="233" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>204</v>
+      </c>
+      <c r="B233">
+        <v>117</v>
+      </c>
+      <c r="C233">
+        <v>207</v>
+      </c>
+      <c r="D233">
+        <v>137</v>
+      </c>
+      <c r="E233">
+        <v>158</v>
+      </c>
+      <c r="F233">
+        <v>123</v>
+      </c>
+      <c r="G233">
+        <v>177</v>
+      </c>
+      <c r="H233">
+        <v>201</v>
+      </c>
+      <c r="I233">
+        <v>179</v>
+      </c>
+      <c r="J233">
+        <v>208</v>
+      </c>
+      <c r="K233">
+        <v>171</v>
+      </c>
+      <c r="L233">
+        <v>180</v>
+      </c>
+      <c r="M233">
+        <v>141</v>
+      </c>
+      <c r="N233">
+        <v>119</v>
+      </c>
+      <c r="O233">
+        <v>106</v>
+      </c>
+      <c r="P233">
+        <v>209</v>
+      </c>
+      <c r="Q233">
+        <v>174</v>
+      </c>
+      <c r="R233">
+        <v>170</v>
+      </c>
+      <c r="S233">
+        <v>176</v>
+      </c>
+      <c r="T233">
+        <v>178</v>
+      </c>
+      <c r="U233">
+        <v>210</v>
+      </c>
+      <c r="V233">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="234" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>117</v>
+      </c>
+      <c r="B234">
+        <v>119</v>
+      </c>
+      <c r="C234">
+        <v>137</v>
+      </c>
+      <c r="D234">
+        <v>106</v>
+      </c>
+      <c r="E234">
+        <v>170</v>
+      </c>
+      <c r="F234">
+        <v>208</v>
+      </c>
+      <c r="G234">
+        <v>211</v>
+      </c>
+      <c r="H234">
+        <v>180</v>
+      </c>
+      <c r="I234">
+        <v>144</v>
+      </c>
+      <c r="J234">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="235" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>118</v>
+      </c>
+      <c r="B235">
+        <v>20</v>
+      </c>
+      <c r="C235">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="236" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>119</v>
+      </c>
+      <c r="B236">
+        <v>129</v>
+      </c>
+      <c r="C236">
+        <v>137</v>
+      </c>
+      <c r="D236">
+        <v>158</v>
+      </c>
+      <c r="E236">
+        <v>170</v>
+      </c>
+      <c r="F236">
+        <v>200</v>
+      </c>
+      <c r="G236">
+        <v>174</v>
+      </c>
+      <c r="H236">
+        <v>120</v>
+      </c>
+      <c r="I236">
+        <v>212</v>
+      </c>
+      <c r="J236">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="237" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>132</v>
+      </c>
+      <c r="B237">
+        <v>120</v>
+      </c>
+      <c r="C237">
+        <v>106</v>
+      </c>
+      <c r="D237">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="238" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>120</v>
+      </c>
+      <c r="B238">
+        <v>106</v>
+      </c>
+      <c r="C238">
+        <v>144</v>
+      </c>
+      <c r="D238">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="239" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>133</v>
+      </c>
+      <c r="B239">
+        <v>166</v>
+      </c>
+      <c r="C239">
+        <v>167</v>
+      </c>
+      <c r="D239">
+        <v>168</v>
+      </c>
+      <c r="E239">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="240" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>134</v>
+      </c>
+      <c r="B240">
+        <v>166</v>
+      </c>
+      <c r="C240">
+        <v>168</v>
+      </c>
+      <c r="D240">
+        <v>187</v>
+      </c>
+      <c r="E240">
+        <v>214</v>
+      </c>
+      <c r="F240">
+        <v>215</v>
+      </c>
+      <c r="G240">
+        <v>216</v>
+      </c>
+      <c r="H240">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>135</v>
+      </c>
+      <c r="B241">
+        <v>167</v>
+      </c>
+      <c r="C241">
+        <v>168</v>
+      </c>
+      <c r="D241">
+        <v>187</v>
+      </c>
+      <c r="E241">
+        <v>166</v>
+      </c>
+      <c r="F241">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>136</v>
+      </c>
+      <c r="B242">
+        <v>166</v>
+      </c>
+      <c r="C242">
+        <v>187</v>
+      </c>
+      <c r="D242">
+        <v>169</v>
+      </c>
+      <c r="E242">
+        <v>168</v>
+      </c>
+      <c r="F242">
+        <v>216</v>
+      </c>
+      <c r="G242">
+        <v>164</v>
+      </c>
+      <c r="H242">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>137</v>
+      </c>
+      <c r="B243">
+        <v>106</v>
+      </c>
+      <c r="C243">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>138</v>
+      </c>
+      <c r="B244">
+        <v>121</v>
+      </c>
+      <c r="C244">
+        <v>217</v>
+      </c>
+      <c r="D244">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>139</v>
+      </c>
+      <c r="B245">
+        <v>169</v>
+      </c>
+      <c r="C245">
+        <v>215</v>
+      </c>
+      <c r="D245">
+        <v>171</v>
+      </c>
+      <c r="E245">
+        <v>187</v>
+      </c>
+      <c r="F245">
+        <v>166</v>
+      </c>
+      <c r="G245">
+        <v>218</v>
+      </c>
+      <c r="H245">
+        <v>219</v>
+      </c>
+      <c r="I245">
+        <v>220</v>
+      </c>
+      <c r="J245">
+        <v>221</v>
+      </c>
+      <c r="K245">
+        <v>188</v>
+      </c>
+      <c r="L245">
+        <v>168</v>
+      </c>
+      <c r="M245">
+        <v>222</v>
+      </c>
+      <c r="N245">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>140</v>
+      </c>
+      <c r="B246">
+        <v>171</v>
+      </c>
+      <c r="C246">
+        <v>187</v>
+      </c>
+      <c r="D246">
+        <v>166</v>
+      </c>
+      <c r="E246">
+        <v>218</v>
+      </c>
+      <c r="F246">
+        <v>219</v>
+      </c>
+      <c r="G246">
+        <v>220</v>
+      </c>
+      <c r="H246">
+        <v>221</v>
+      </c>
+      <c r="I246">
+        <v>188</v>
+      </c>
+      <c r="J246">
+        <v>168</v>
+      </c>
+      <c r="K246">
+        <v>222</v>
+      </c>
+      <c r="L246">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>142</v>
+      </c>
+      <c r="B248">
+        <v>215</v>
+      </c>
+      <c r="C248">
+        <v>187</v>
+      </c>
+      <c r="D248">
+        <v>168</v>
+      </c>
+      <c r="E248">
+        <v>223</v>
+      </c>
+      <c r="F248">
+        <v>224</v>
+      </c>
+      <c r="G248">
+        <v>225</v>
+      </c>
+      <c r="H248">
+        <v>226</v>
+      </c>
+      <c r="I248">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>143</v>
+      </c>
+      <c r="B249">
+        <v>187</v>
+      </c>
+      <c r="C249">
+        <v>168</v>
+      </c>
+      <c r="D249">
+        <v>169</v>
+      </c>
+      <c r="E249">
+        <v>142</v>
+      </c>
+      <c r="F249">
+        <v>164</v>
+      </c>
+      <c r="G249">
+        <v>163</v>
+      </c>
+      <c r="H249">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>144</v>
+      </c>
+      <c r="B250">
+        <v>200</v>
+      </c>
+      <c r="C250">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>145</v>
+      </c>
+      <c r="B251">
+        <v>138</v>
+      </c>
+      <c r="C251">
+        <v>213</v>
+      </c>
+      <c r="D251">
+        <v>179</v>
+      </c>
+      <c r="E251">
+        <v>180</v>
+      </c>
+      <c r="F251">
+        <v>174</v>
+      </c>
+      <c r="G251">
+        <v>228</v>
+      </c>
+      <c r="H251">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>146</v>
+      </c>
+      <c r="B252">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>148</v>
+      </c>
+      <c r="B254">
+        <v>149</v>
+      </c>
+      <c r="C254">
+        <v>147</v>
+      </c>
+      <c r="D254">
+        <v>146</v>
+      </c>
+      <c r="E254">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>149</v>
+      </c>
+      <c r="B255">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>150</v>
+      </c>
+      <c r="B256">
+        <v>229</v>
+      </c>
+      <c r="C256">
+        <v>222</v>
+      </c>
+      <c r="D256">
+        <v>219</v>
+      </c>
+      <c r="E256">
+        <v>188</v>
+      </c>
+      <c r="F256">
+        <v>230</v>
+      </c>
+      <c r="G256">
+        <v>231</v>
+      </c>
+      <c r="H256">
+        <v>171</v>
+      </c>
+      <c r="I256">
+        <v>187</v>
+      </c>
+      <c r="J256">
+        <v>151</v>
+      </c>
+      <c r="K256">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="257" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>151</v>
+      </c>
+      <c r="B257">
+        <v>229</v>
+      </c>
+      <c r="C257">
+        <v>222</v>
+      </c>
+      <c r="D257">
+        <v>219</v>
+      </c>
+      <c r="E257">
+        <v>188</v>
+      </c>
+      <c r="F257">
+        <v>230</v>
+      </c>
+      <c r="G257">
+        <v>231</v>
+      </c>
+      <c r="H257">
+        <v>171</v>
+      </c>
+      <c r="I257">
+        <v>187</v>
+      </c>
+      <c r="J257">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="258" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>152</v>
+      </c>
+      <c r="B258">
+        <v>166</v>
+      </c>
+      <c r="C258">
+        <v>187</v>
+      </c>
+      <c r="D258">
+        <v>171</v>
+      </c>
+      <c r="E258">
+        <v>215</v>
+      </c>
+      <c r="F258">
+        <v>230</v>
+      </c>
+      <c r="G258">
+        <v>218</v>
+      </c>
+      <c r="H258">
+        <v>169</v>
+      </c>
+      <c r="I258">
+        <v>237</v>
+      </c>
+      <c r="J258">
+        <v>229</v>
+      </c>
+      <c r="K258">
+        <v>232</v>
+      </c>
+      <c r="L258">
+        <v>233</v>
+      </c>
+      <c r="M258">
+        <v>0</v>
+      </c>
+      <c r="N258">
+        <v>235</v>
+      </c>
+      <c r="O258">
+        <v>236</v>
+      </c>
+      <c r="P258">
+        <v>168</v>
+      </c>
+      <c r="Q258">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="259" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>153</v>
+      </c>
+      <c r="B259">
+        <v>169</v>
+      </c>
+      <c r="C259">
+        <v>216</v>
+      </c>
+      <c r="D259">
+        <v>218</v>
+      </c>
+      <c r="E259">
+        <v>238</v>
+      </c>
+      <c r="F259">
+        <v>168</v>
+      </c>
+      <c r="G259">
+        <v>215</v>
+      </c>
+      <c r="H259">
+        <v>187</v>
+      </c>
+      <c r="I259">
+        <v>166</v>
+      </c>
+      <c r="J259">
+        <v>163</v>
+      </c>
+      <c r="K259">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="260" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>154</v>
+      </c>
+      <c r="B260">
+        <v>240</v>
+      </c>
+      <c r="C260">
+        <v>187</v>
+      </c>
+      <c r="D260">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="261" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>155</v>
+      </c>
+      <c r="B261">
+        <v>187</v>
+      </c>
+      <c r="C261">
+        <v>167</v>
+      </c>
+      <c r="D261">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="262" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>156</v>
+      </c>
+      <c r="B262">
+        <v>167</v>
+      </c>
+      <c r="C262">
+        <v>166</v>
+      </c>
+      <c r="D262">
+        <v>187</v>
+      </c>
+      <c r="E262">
+        <v>168</v>
+      </c>
+      <c r="F262">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="263" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>157</v>
+      </c>
+      <c r="B263">
+        <v>188</v>
+      </c>
+      <c r="C263">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="264" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>158</v>
+      </c>
+      <c r="B264">
+        <v>166</v>
+      </c>
+      <c r="C264">
+        <v>187</v>
+      </c>
+      <c r="D264">
+        <v>168</v>
+      </c>
+      <c r="E264">
+        <v>188</v>
+      </c>
+      <c r="F264">
+        <v>241</v>
+      </c>
+      <c r="G264">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="265" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>159</v>
+      </c>
+      <c r="B265">
+        <v>236</v>
+      </c>
+      <c r="C265">
+        <v>169</v>
+      </c>
+      <c r="D265">
+        <v>187</v>
+      </c>
+      <c r="E265">
+        <v>223</v>
+      </c>
+      <c r="F265">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="266" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A266">
+        <v>160</v>
+      </c>
+      <c r="B266">
+        <v>168</v>
+      </c>
+      <c r="C266">
+        <v>166</v>
+      </c>
+      <c r="D266">
+        <v>187</v>
+      </c>
+      <c r="E266">
+        <v>169</v>
+      </c>
+      <c r="F266">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="267" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A267">
+        <v>161</v>
+      </c>
+      <c r="B267">
+        <v>223</v>
+      </c>
+      <c r="C267">
+        <v>187</v>
+      </c>
+      <c r="D267">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="268" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A268">
+        <v>162</v>
+      </c>
+      <c r="B268">
+        <v>187</v>
+      </c>
+      <c r="C268">
+        <v>168</v>
+      </c>
+      <c r="D268">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="269" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A269">
+        <v>163</v>
+      </c>
+      <c r="B269">
+        <v>166</v>
+      </c>
+      <c r="C269">
+        <v>187</v>
+      </c>
+      <c r="D269">
+        <v>168</v>
+      </c>
+      <c r="E269">
+        <v>169</v>
+      </c>
+      <c r="F269">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="270" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A270">
+        <v>164</v>
+      </c>
+      <c r="B270">
+        <v>166</v>
+      </c>
+      <c r="C270">
+        <v>187</v>
+      </c>
+      <c r="D270">
+        <v>168</v>
+      </c>
+      <c r="E270">
+        <v>169</v>
+      </c>
+      <c r="F270">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="271" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A271">
+        <v>165</v>
+      </c>
+      <c r="B271">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="272" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A272">
+        <v>103</v>
+      </c>
+      <c r="B272">
+        <v>243</v>
+      </c>
+      <c r="C272">
+        <v>121</v>
+      </c>
+      <c r="D272">
+        <v>180</v>
+      </c>
+      <c r="E272">
+        <v>200</v>
+      </c>
+      <c r="F272">
+        <v>179</v>
+      </c>
+      <c r="G272">
+        <v>174</v>
+      </c>
+      <c r="H272">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A273">
+        <v>104</v>
+      </c>
+      <c r="B273">
+        <v>105</v>
+      </c>
+      <c r="C273">
+        <v>106</v>
+      </c>
+      <c r="D273">
+        <v>137</v>
+      </c>
+      <c r="E273">
+        <v>245</v>
+      </c>
+      <c r="F273">
+        <v>223</v>
+      </c>
+      <c r="G273">
+        <v>174</v>
+      </c>
+      <c r="H273">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A274">
+        <v>105</v>
+      </c>
+      <c r="B274">
+        <v>138</v>
+      </c>
+      <c r="C274">
+        <v>189</v>
+      </c>
+      <c r="D274">
+        <v>174</v>
+      </c>
+      <c r="E274">
+        <v>121</v>
+      </c>
+      <c r="F274">
+        <v>180</v>
+      </c>
+      <c r="G274">
+        <v>144</v>
+      </c>
+      <c r="H274">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A275">
+        <v>106</v>
+      </c>
+      <c r="B275">
+        <v>201</v>
+      </c>
+      <c r="C275">
+        <v>180</v>
+      </c>
+      <c r="D275">
+        <v>179</v>
+      </c>
+      <c r="E275">
+        <v>246</v>
+      </c>
+      <c r="F275">
+        <v>144</v>
+      </c>
+      <c r="G275">
+        <v>247</v>
+      </c>
+      <c r="H275">
+        <v>213</v>
+      </c>
+      <c r="I275">
+        <v>228</v>
+      </c>
+      <c r="J275">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A276">
+        <v>107</v>
+      </c>
+      <c r="B276">
+        <v>106</v>
+      </c>
+      <c r="C276">
+        <v>174</v>
+      </c>
+      <c r="D276">
+        <v>180</v>
+      </c>
+      <c r="E276">
+        <v>108</v>
+      </c>
+      <c r="F276">
+        <v>103</v>
+      </c>
+      <c r="G276">
+        <v>243</v>
+      </c>
+      <c r="H276">
+        <v>248</v>
+      </c>
+      <c r="I276">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A277">
+        <v>108</v>
+      </c>
+      <c r="B277">
+        <v>105</v>
+      </c>
+      <c r="C277">
+        <v>106</v>
+      </c>
+      <c r="D277">
+        <v>243</v>
+      </c>
+      <c r="E277">
+        <v>137</v>
+      </c>
+      <c r="F277">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A278">
+        <v>109</v>
+      </c>
+      <c r="B278">
+        <v>110</v>
+      </c>
+      <c r="C278">
+        <v>136</v>
+      </c>
+      <c r="D278">
+        <v>178</v>
+      </c>
+      <c r="E278">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A279">
+        <v>110</v>
+      </c>
+      <c r="B279">
+        <v>177</v>
+      </c>
+      <c r="C279">
+        <v>123</v>
+      </c>
+      <c r="D279">
+        <v>171</v>
+      </c>
+      <c r="E279">
+        <v>180</v>
+      </c>
+      <c r="F279">
+        <v>189</v>
+      </c>
+      <c r="G279">
+        <v>173</v>
+      </c>
+      <c r="H279">
+        <v>174</v>
+      </c>
+      <c r="I279">
+        <v>107</v>
+      </c>
+      <c r="J279">
+        <v>145</v>
+      </c>
+      <c r="K279">
+        <v>141</v>
+      </c>
+      <c r="L279">
+        <v>106</v>
+      </c>
+      <c r="M279">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A280">
+        <v>124</v>
+      </c>
+      <c r="B280">
+        <v>7</v>
+      </c>
+      <c r="C280">
+        <v>8</v>
+      </c>
+      <c r="D280">
+        <v>9</v>
+      </c>
+      <c r="E280">
+        <v>10</v>
+      </c>
+      <c r="F280">
+        <v>11</v>
+      </c>
+      <c r="G280">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A281">
+        <v>114</v>
+      </c>
+      <c r="B281">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A282">
+        <v>110</v>
+      </c>
+      <c r="B282">
+        <v>18</v>
+      </c>
+      <c r="C282">
+        <v>19</v>
+      </c>
+      <c r="D282">
+        <v>22</v>
+      </c>
+      <c r="E282">
+        <v>23</v>
+      </c>
+      <c r="F282">
+        <v>24</v>
+      </c>
+      <c r="G282">
+        <v>25</v>
+      </c>
+      <c r="H282">
+        <v>26</v>
+      </c>
+      <c r="I282">
+        <v>27</v>
+      </c>
+      <c r="J282">
+        <v>28</v>
+      </c>
+      <c r="K282">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A283">
+        <v>106</v>
+      </c>
+      <c r="B283">
+        <v>20</v>
+      </c>
+      <c r="C283">
+        <v>21</v>
+      </c>
+      <c r="D283">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A284">
+        <v>129</v>
+      </c>
+      <c r="B284">
+        <v>31</v>
+      </c>
+      <c r="C284">
+        <v>32</v>
+      </c>
+      <c r="D284">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>